<commit_message>
update UI, submission reports
</commit_message>
<xml_diff>
--- a/documents/test_data/test_v4_no_date.xlsx
+++ b/documents/test_data/test_v4_no_date.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lonnemanm\Documents\Repositories\data_portal\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlonn\Documents\Repositories\data_portal\documents\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA75089-E9E2-412E-A223-4E4AF0A0538D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4EAF2C-BBF3-4DF7-9712-6CCF5005B676}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="protocol_metadata" sheetId="1" r:id="rId1"/>
@@ -1347,7 +1347,7 @@
   </sheetPr>
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1506,9 +1506,9 @@
   </sheetPr>
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1573,7 +1573,9 @@
       <c r="C2" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D2" s="14"/>
+      <c r="D2" s="14">
+        <v>1</v>
+      </c>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:12">
@@ -1586,7 +1588,9 @@
       <c r="C3" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D3" s="14"/>
+      <c r="D3" s="14">
+        <v>2</v>
+      </c>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:12">
@@ -1599,7 +1603,9 @@
       <c r="C4" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D4" s="14"/>
+      <c r="D4" s="14">
+        <v>3</v>
+      </c>
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:12">

</xml_diff>